<commit_message>
graphs for performance and rt
</commit_message>
<xml_diff>
--- a/Checking performance and rt.xlsx
+++ b/Checking performance and rt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joce\Documents\Jocelyn\PolyU RA\collab-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jocel\Documents\Collab project Marco Pang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE738BC-C433-4AF3-B793-3A2685C6BAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D633CBFE-C1CD-4586-B959-D08B539DA141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,6 +151,499 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>206375</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1DB45C4-8044-47F5-83AD-94331E3031F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="6586536"/>
+          <a:ext cx="4540250" cy="3405189"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{774014A3-D187-49FA-A66C-40B909669555}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15563850" y="6600824"/>
+          <a:ext cx="4572000" cy="3429000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2C163EB-27DC-40A1-BEEE-1812D247AE34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10629900" y="6524625"/>
+          <a:ext cx="4648200" cy="3486150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>59530</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DEA0CC8-B617-4128-A227-69D1EE3B126C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5276850" y="6572249"/>
+          <a:ext cx="4524375" cy="3393281"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4CE95F5-DC60-465E-B022-E6F2BCC8177A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15116175" y="2162175"/>
+          <a:ext cx="4660900" cy="3495675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>164306</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05E88439-8BA4-415B-BFB9-315B9F4B3AB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10325099" y="2181225"/>
+          <a:ext cx="4676775" cy="3507581"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>587375</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1F77C34-B281-45BF-901F-1D4174F03A27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5391150" y="2124075"/>
+          <a:ext cx="4826000" cy="3619500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>169069</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2001F85-F9F9-4E98-B046-324AD4C80E74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="2095500"/>
+          <a:ext cx="4543425" cy="3407569"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -416,19 +909,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U34"/>
+  <dimension ref="A1:AA34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:27">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -445,7 +939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -458,15 +952,15 @@
         <v>0.82500000000000007</v>
       </c>
       <c r="D2">
-        <f>AVERAGE(O9:O11)</f>
+        <f>AVERAGE(T9:T11)</f>
         <v>0.69166666666666676</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(U9:U11)</f>
+        <f>AVERAGE(AA9:AA11)</f>
         <v>0.71666666666666679</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -479,33 +973,33 @@
         <v>1.4835397411756868</v>
       </c>
       <c r="D3">
-        <f>AVERAGE(M32:M34)</f>
+        <f>AVERAGE(R32:R34)</f>
         <v>0.96099349570133663</v>
       </c>
       <c r="E3">
-        <f>AVERAGE(S32:S34)</f>
-        <v>0.8973432240212077</v>
+        <f>AVERAGE(Z32:Z34)</f>
+        <v>0.89863720718502504</v>
       </c>
       <c r="F3">
         <f>AVERAGE(0.8976, 1.1133, 1.6361)</f>
         <v>1.2156666666666667</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:27">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J7" t="s">
         <v>6</v>
       </c>
-      <c r="L7" t="s">
+      <c r="Q7" t="s">
         <v>12</v>
       </c>
-      <c r="R7" t="s">
+      <c r="X7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:27">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -515,35 +1009,35 @@
       <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
+      <c r="J8" t="s">
         <v>17</v>
       </c>
-      <c r="H8" t="s">
+      <c r="K8" t="s">
         <v>16</v>
       </c>
-      <c r="I8" t="s">
+      <c r="L8" t="s">
         <v>18</v>
       </c>
-      <c r="L8" t="s">
+      <c r="Q8" t="s">
         <v>17</v>
       </c>
-      <c r="M8" t="s">
+      <c r="R8" t="s">
         <v>16</v>
       </c>
-      <c r="N8" t="s">
+      <c r="S8" t="s">
         <v>18</v>
       </c>
-      <c r="R8" t="s">
+      <c r="X8" t="s">
         <v>17</v>
       </c>
-      <c r="S8" t="s">
+      <c r="Y8" t="s">
         <v>16</v>
       </c>
-      <c r="T8" t="s">
+      <c r="Z8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:27">
       <c r="A9">
         <v>1</v>
       </c>
@@ -556,52 +1050,52 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="I9">
         <v>1</v>
       </c>
-      <c r="G9">
+      <c r="J9">
         <v>66</v>
       </c>
-      <c r="H9">
+      <c r="K9">
         <v>11</v>
       </c>
-      <c r="I9">
+      <c r="L9">
         <v>3</v>
       </c>
-      <c r="K9">
+      <c r="P9">
         <v>1</v>
       </c>
-      <c r="L9">
+      <c r="Q9">
         <v>52</v>
       </c>
-      <c r="M9">
+      <c r="R9">
         <v>25</v>
       </c>
-      <c r="N9">
+      <c r="S9">
         <v>3</v>
       </c>
-      <c r="O9">
+      <c r="T9">
         <f>52/80</f>
         <v>0.65</v>
       </c>
-      <c r="Q9">
+      <c r="W9">
         <v>1</v>
       </c>
-      <c r="R9">
+      <c r="X9">
         <v>61</v>
       </c>
-      <c r="S9">
+      <c r="Y9">
         <v>16</v>
       </c>
-      <c r="T9">
+      <c r="Z9">
         <v>3</v>
       </c>
-      <c r="U9">
+      <c r="AA9">
         <f>61/80</f>
         <v>0.76249999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:27">
       <c r="A10">
         <v>2</v>
       </c>
@@ -614,52 +1108,52 @@
       <c r="D10">
         <v>2</v>
       </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10">
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
         <v>70</v>
       </c>
-      <c r="H10">
+      <c r="K10">
         <v>10</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <v>0</v>
       </c>
-      <c r="K10">
-        <v>2</v>
-      </c>
-      <c r="L10">
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10">
         <v>54</v>
       </c>
-      <c r="M10">
+      <c r="R10">
         <v>26</v>
       </c>
-      <c r="N10">
+      <c r="S10">
         <v>0</v>
       </c>
-      <c r="O10">
+      <c r="T10">
         <f>54/80</f>
         <v>0.67500000000000004</v>
       </c>
-      <c r="Q10">
-        <v>2</v>
-      </c>
-      <c r="R10">
+      <c r="W10">
+        <v>2</v>
+      </c>
+      <c r="X10">
         <v>62</v>
       </c>
-      <c r="S10">
+      <c r="Y10">
         <v>18</v>
       </c>
-      <c r="T10">
+      <c r="Z10">
         <v>0</v>
       </c>
-      <c r="U10">
+      <c r="AA10">
         <f>62/80</f>
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:27">
       <c r="A11">
         <v>3</v>
       </c>
@@ -672,150 +1166,157 @@
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="F11">
+      <c r="I11">
         <v>3</v>
       </c>
-      <c r="G11">
+      <c r="J11">
         <v>62</v>
       </c>
-      <c r="H11">
+      <c r="K11">
         <v>6</v>
       </c>
-      <c r="I11">
+      <c r="L11">
         <v>12</v>
       </c>
-      <c r="K11">
+      <c r="P11">
         <v>3</v>
       </c>
-      <c r="L11">
+      <c r="Q11">
         <v>60</v>
       </c>
-      <c r="M11">
+      <c r="R11">
         <v>20</v>
       </c>
-      <c r="N11">
+      <c r="S11">
         <v>0</v>
       </c>
-      <c r="O11">
+      <c r="T11">
         <f>60/80</f>
         <v>0.75</v>
       </c>
-      <c r="Q11">
+      <c r="W11">
         <v>3</v>
       </c>
-      <c r="R11">
+      <c r="X11">
         <v>49</v>
       </c>
-      <c r="S11">
+      <c r="Y11">
         <v>29</v>
       </c>
-      <c r="T11">
-        <v>2</v>
-      </c>
-      <c r="U11">
+      <c r="Z11">
+        <v>2</v>
+      </c>
+      <c r="AA11">
         <f>49/80</f>
         <v>0.61250000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:26">
       <c r="A30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:26">
       <c r="A31" t="s">
         <v>7</v>
       </c>
-      <c r="G31" t="s">
+      <c r="J31" t="s">
         <v>8</v>
       </c>
-      <c r="L31" t="s">
+      <c r="Q31" t="s">
         <v>11</v>
       </c>
-      <c r="R31" t="s">
+      <c r="Y31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:26">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32">
         <v>1.03777219073769</v>
       </c>
-      <c r="G32">
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="J32">
         <v>1</v>
       </c>
-      <c r="H32">
+      <c r="K32">
         <v>1.38742181558355</v>
       </c>
-      <c r="L32">
+      <c r="Q32">
         <v>1</v>
       </c>
-      <c r="M32" s="1">
+      <c r="R32" s="1">
         <v>0.969171688362786</v>
       </c>
-      <c r="R32">
+      <c r="Y32">
         <v>1</v>
       </c>
-      <c r="S32" s="1">
+      <c r="Z32" s="1">
         <v>1.01479018187035</v>
       </c>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:26">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33">
         <v>0.79001045193993202</v>
       </c>
-      <c r="G33">
-        <v>2</v>
-      </c>
-      <c r="H33">
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33">
         <v>1.4229372300000001</v>
       </c>
-      <c r="L33">
-        <v>2</v>
-      </c>
-      <c r="M33">
+      <c r="Q33">
+        <v>2</v>
+      </c>
+      <c r="R33">
         <v>0.733829582489124</v>
       </c>
-      <c r="R33">
-        <v>2</v>
-      </c>
-      <c r="S33" s="1">
+      <c r="Y33">
+        <v>2</v>
+      </c>
+      <c r="Z33" s="1">
         <v>0.78248423249970001</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:26">
       <c r="A34">
         <v>3</v>
       </c>
       <c r="B34">
         <v>0.88521696132374705</v>
       </c>
-      <c r="G34">
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="J34">
         <v>3</v>
       </c>
-      <c r="H34">
+      <c r="K34">
         <v>1.64026017794351</v>
       </c>
-      <c r="L34">
+      <c r="Q34">
         <v>3</v>
       </c>
-      <c r="M34">
+      <c r="R34">
         <v>1.1799792162520999</v>
       </c>
-      <c r="R34">
+      <c r="Y34">
         <v>3</v>
-      </c>
-      <c r="S34" s="1">
-        <v>0.894755257693573</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>